<commit_message>
last version in laptop
</commit_message>
<xml_diff>
--- a/expriment/main/AFFPrac.xlsx
+++ b/expriment/main/AFFPrac.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ryougi mana\Desktop\CF_DDM\expriment\main\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70650D65-F98B-4211-A048-C3D70A12975D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26DE1C16-0DAE-41A5-9D1F-70D2152A8F0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="24">
   <si>
     <t>congruency</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -108,13 +108,11 @@
     <t>s</t>
   </si>
   <si>
+    <t>a</t>
+  </si>
+  <si>
     <t>k</t>
-  </si>
-  <si>
-    <t>a</t>
-  </si>
-  <si>
-    <t>l</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -442,7 +440,7 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -491,7 +489,7 @@
         <v>21</v>
       </c>
       <c r="F2" t="s">
-        <v>22</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -508,10 +506,10 @@
         <v>18</v>
       </c>
       <c r="E3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F3" t="s">
         <v>23</v>
-      </c>
-      <c r="F3" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -528,10 +526,10 @@
         <v>18</v>
       </c>
       <c r="E4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F4" t="s">
-        <v>22</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -551,7 +549,7 @@
         <v>21</v>
       </c>
       <c r="F5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -568,10 +566,10 @@
         <v>19</v>
       </c>
       <c r="E6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F6" t="s">
-        <v>22</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -591,7 +589,7 @@
         <v>21</v>
       </c>
       <c r="F7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
@@ -611,7 +609,7 @@
         <v>21</v>
       </c>
       <c r="F8" t="s">
-        <v>22</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
@@ -628,10 +626,10 @@
         <v>19</v>
       </c>
       <c r="E9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F9" t="s">
         <v>23</v>
-      </c>
-      <c r="F9" t="s">
-        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>